<commit_message>
Matching saledata w/ sn
</commit_message>
<xml_diff>
--- a/product_names.xlsx
+++ b/product_names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pies6\Desktop\DSMedi_server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D3EA8A-4682-4D14-819A-9BA2CF84D6B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF19620-BEC8-4D66-B10B-3350A938165B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="1395" windowWidth="25335" windowHeight="13065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>바로잰 혈당측정지(스트립)</t>
   </si>
@@ -57,17 +57,21 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>erp_code</t>
+    <t>3534</t>
+  </si>
+  <si>
+    <t>00953</t>
+  </si>
+  <si>
+    <t>00753</t>
+  </si>
+  <si>
+    <t>erp_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3534</t>
-  </si>
-  <si>
-    <t>00953</t>
-  </si>
-  <si>
-    <t>00753</t>
+    <t>mall_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -130,13 +134,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -418,30 +428,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="43.75" customWidth="1"/>
-    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="2" max="2" width="15.125" customWidth="1"/>
+    <col min="3" max="3" width="71.875" customWidth="1"/>
+    <col min="4" max="4" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -451,67 +465,86 @@
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="3">
+        <v>45371</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="4">
+        <v>101716</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="4">
+        <v>104968</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="4">
+        <v>105250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="3">
+        <v>104192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="3">
+        <v>108075</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C12" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>